<commit_message>
Update Radio/TV (Life and living), CD/VHS
</commit_message>
<xml_diff>
--- a/프좀 용어집.xlsx
+++ b/프좀 용어집.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF1DFD8-145A-4D7D-8257-E693D779C6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2478D53B-FB9D-4254-A611-DE180D33F780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3576" yWindow="696" windowWidth="17280" windowHeight="10728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3576" yWindow="696" windowWidth="17280" windowHeight="10728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="라디오,TV" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="981">
   <si>
     <t>종류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3869,6 +3869,10 @@
   </si>
   <si>
     <t>오늘 밤 함께해 주셔서 감사합니다. 질서정연하고 책임감 있는 언론의 역할 부탁드립니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~~주다 띄어쓰기 통일 안 된 상태임(띄어쓰기 원칙 붙임 허용)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4322,8 +4326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="AE1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AP15" sqref="AP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -7699,10 +7703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -7823,6 +7827,11 @@
       <c r="H15" s="2">
         <f>H14/H13</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Radio/TV (TURBO), CD/VHS
</commit_message>
<xml_diff>
--- a/프좀 용어집.xlsx
+++ b/프좀 용어집.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2478D53B-FB9D-4254-A611-DE180D33F780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947F0006-2F6F-4D4A-863E-B0CEE5BC7901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3576" yWindow="696" windowWidth="17280" windowHeight="10728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3576" yWindow="696" windowWidth="17280" windowHeight="10728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="라디오,TV" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="991">
   <si>
     <t>종류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3787,10 +3787,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>트리플-N 클로징 멘트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>대통령 성명(2차)(대규모 폭력 사태 이후)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3873,6 +3869,48 @@
   </si>
   <si>
     <t>~~주다 띄어쓰기 통일 안 된 상태임(띄어쓰기 원칙 붙임 허용)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>터보, 당신의 친구. 당신의 오락!</t>
+  </si>
+  <si>
+    <t>TURBO: Your friend. Your entertainment!</t>
+  </si>
+  <si>
+    <t>터보 오프닝 대사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트리플-N 클로징 대사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tinsel Town</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틴셀타운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할리우드의 별칭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hollywood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할리우드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3972,10 +4010,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표1" displayName="표1" ref="A1:D187" totalsRowShown="0">
-  <autoFilter ref="A1:D187" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D187">
-    <sortCondition ref="A1:A187"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표1" displayName="표1" ref="A1:D190" totalsRowShown="0">
+  <autoFilter ref="A1:D190" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D190">
+    <sortCondition ref="A1:A190"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="종류"/>
@@ -4324,10 +4362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CP187"/>
+  <dimension ref="A1:CP190"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AP15" sqref="AP15"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4378,7 +4416,7 @@
         <v>298</v>
       </c>
       <c r="AP2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="AY2" t="s">
         <v>392</v>
@@ -5063,7 +5101,7 @@
         <v>956</v>
       </c>
       <c r="D19" t="s">
-        <v>957</v>
+        <v>984</v>
       </c>
       <c r="F19" t="s">
         <v>100</v>
@@ -5098,13 +5136,13 @@
         <v>950</v>
       </c>
       <c r="B20" t="s">
+        <v>965</v>
+      </c>
+      <c r="C20" t="s">
         <v>966</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>967</v>
-      </c>
-      <c r="D20" t="s">
-        <v>968</v>
       </c>
       <c r="F20" t="s">
         <v>101</v>
@@ -5139,7 +5177,7 @@
         <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="D21" t="s">
         <v>285</v>
@@ -5180,13 +5218,13 @@
         <v>950</v>
       </c>
       <c r="B22" t="s">
+        <v>963</v>
+      </c>
+      <c r="C22" t="s">
         <v>964</v>
       </c>
-      <c r="C22" t="s">
-        <v>965</v>
-      </c>
       <c r="D22" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="AH22" t="s">
         <v>322</v>
@@ -5247,16 +5285,16 @@
     </row>
     <row r="24" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
+        <v>970</v>
+      </c>
+      <c r="B24" t="s">
+        <v>972</v>
+      </c>
+      <c r="C24" t="s">
         <v>971</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>973</v>
-      </c>
-      <c r="C24" t="s">
-        <v>972</v>
-      </c>
-      <c r="D24" t="s">
-        <v>974</v>
       </c>
       <c r="F24" t="s">
         <v>104</v>
@@ -5288,16 +5326,16 @@
     </row>
     <row r="25" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B25" t="s">
+        <v>974</v>
+      </c>
+      <c r="C25" t="s">
+        <v>976</v>
+      </c>
+      <c r="D25" t="s">
         <v>975</v>
-      </c>
-      <c r="C25" t="s">
-        <v>977</v>
-      </c>
-      <c r="D25" t="s">
-        <v>976</v>
       </c>
       <c r="F25" t="s">
         <v>105</v>
@@ -5332,13 +5370,13 @@
         <v>950</v>
       </c>
       <c r="B26" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C26" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D26" t="s">
-        <v>957</v>
+        <v>984</v>
       </c>
       <c r="AH26" t="s">
         <v>325</v>
@@ -5395,84 +5433,57 @@
     </row>
     <row r="29" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>618</v>
+        <v>980</v>
       </c>
       <c r="B29" t="s">
-        <v>659</v>
+        <v>982</v>
       </c>
       <c r="C29" t="s">
-        <v>660</v>
+        <v>981</v>
       </c>
       <c r="D29" t="s">
-        <v>621</v>
-      </c>
-      <c r="F29" t="s">
-        <v>106</v>
-      </c>
-      <c r="N29" t="s">
-        <v>350</v>
-      </c>
-      <c r="AH29" t="s">
-        <v>328</v>
-      </c>
-      <c r="AP29" t="s">
-        <v>383</v>
-      </c>
-      <c r="AY29" t="s">
-        <v>415</v>
-      </c>
-      <c r="BH29" t="s">
-        <v>442</v>
-      </c>
-      <c r="BQ29" t="s">
-        <v>979</v>
-      </c>
-      <c r="CI29" t="s">
-        <v>507</v>
-      </c>
-      <c r="CP29" t="s">
-        <v>543</v>
+        <v>983</v>
       </c>
     </row>
     <row r="30" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>719</v>
+        <v>618</v>
       </c>
       <c r="B30" t="s">
-        <v>747</v>
+        <v>659</v>
       </c>
       <c r="C30" t="s">
-        <v>748</v>
+        <v>660</v>
       </c>
       <c r="D30" t="s">
-        <v>749</v>
+        <v>621</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AH30" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="AP30" t="s">
-        <v>510</v>
+        <v>383</v>
       </c>
       <c r="AY30" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="BH30" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="BQ30" t="s">
-        <v>471</v>
+        <v>978</v>
       </c>
       <c r="CI30" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="CP30" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="31" spans="1:94" x14ac:dyDescent="0.4">
@@ -5480,734 +5491,761 @@
         <v>719</v>
       </c>
       <c r="B31" t="s">
-        <v>720</v>
+        <v>747</v>
       </c>
       <c r="C31" t="s">
-        <v>721</v>
+        <v>748</v>
       </c>
       <c r="D31" t="s">
-        <v>722</v>
+        <v>749</v>
       </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N31" t="s">
-        <v>352</v>
+        <v>351</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>354</v>
       </c>
       <c r="AP31" t="s">
-        <v>961</v>
+        <v>510</v>
+      </c>
+      <c r="AY31" t="s">
+        <v>416</v>
       </c>
       <c r="BH31" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="BQ31" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="CI31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="CP31" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="32" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>618</v>
+        <v>719</v>
       </c>
       <c r="B32" t="s">
-        <v>627</v>
+        <v>720</v>
       </c>
       <c r="C32" t="s">
-        <v>628</v>
+        <v>721</v>
       </c>
       <c r="D32" t="s">
-        <v>621</v>
+        <v>722</v>
       </c>
       <c r="F32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AP32" t="s">
-        <v>385</v>
+        <v>960</v>
       </c>
       <c r="BH32" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="BQ32" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="CI32" t="s">
-        <v>497</v>
+        <v>509</v>
       </c>
       <c r="CP32" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="33" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>673</v>
+        <v>618</v>
       </c>
       <c r="B33" t="s">
-        <v>688</v>
+        <v>627</v>
       </c>
       <c r="C33" t="s">
-        <v>689</v>
+        <v>628</v>
       </c>
       <c r="D33" t="s">
         <v>621</v>
       </c>
       <c r="F33" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="N33" t="s">
+        <v>353</v>
       </c>
       <c r="AP33" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="BH33" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="BQ33" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="CI33" t="s">
         <v>497</v>
       </c>
       <c r="CP33" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="34" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>618</v>
+        <v>673</v>
       </c>
       <c r="B34" t="s">
-        <v>629</v>
+        <v>688</v>
       </c>
       <c r="C34" t="s">
-        <v>630</v>
+        <v>689</v>
       </c>
       <c r="D34" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="F34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AP34" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="BH34" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="BQ34" t="s">
-        <v>474</v>
+        <v>488</v>
       </c>
       <c r="CI34" t="s">
         <v>497</v>
       </c>
       <c r="CP34" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="35" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>673</v>
+        <v>618</v>
       </c>
       <c r="B35" t="s">
-        <v>684</v>
+        <v>629</v>
       </c>
       <c r="C35" t="s">
-        <v>685</v>
+        <v>630</v>
       </c>
       <c r="D35" t="s">
-        <v>621</v>
+        <v>631</v>
       </c>
       <c r="F35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AP35" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="BH35" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="BQ35" t="s">
-        <v>475</v>
+        <v>474</v>
+      </c>
+      <c r="CI35" t="s">
+        <v>497</v>
       </c>
       <c r="CP35" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="36" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>618</v>
+        <v>673</v>
       </c>
       <c r="B36" t="s">
-        <v>647</v>
+        <v>684</v>
       </c>
       <c r="C36" t="s">
-        <v>648</v>
+        <v>685</v>
       </c>
       <c r="D36" t="s">
         <v>621</v>
       </c>
       <c r="F36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AP36" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="BH36" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="BQ36" t="s">
-        <v>476</v>
+        <v>475</v>
+      </c>
+      <c r="CP36" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="37" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>673</v>
+        <v>618</v>
       </c>
       <c r="B37" t="s">
-        <v>678</v>
+        <v>647</v>
       </c>
       <c r="C37" t="s">
-        <v>679</v>
+        <v>648</v>
       </c>
       <c r="D37" t="s">
         <v>621</v>
       </c>
+      <c r="F37" t="s">
+        <v>113</v>
+      </c>
       <c r="AP37" t="s">
-        <v>390</v>
+        <v>389</v>
+      </c>
+      <c r="BH37" t="s">
+        <v>449</v>
       </c>
       <c r="BQ37" t="s">
-        <v>477</v>
-      </c>
-      <c r="CP37" t="s">
-        <v>556</v>
+        <v>476</v>
       </c>
     </row>
     <row r="38" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>852</v>
+        <v>673</v>
       </c>
       <c r="B38" t="s">
-        <v>866</v>
+        <v>678</v>
       </c>
       <c r="C38" t="s">
-        <v>867</v>
+        <v>679</v>
       </c>
       <c r="D38" t="s">
-        <v>868</v>
+        <v>621</v>
       </c>
       <c r="AP38" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="BQ38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="CP38" t="s">
-        <v>595</v>
+        <v>556</v>
       </c>
     </row>
     <row r="39" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>618</v>
+        <v>852</v>
       </c>
       <c r="B39" t="s">
-        <v>643</v>
+        <v>866</v>
       </c>
       <c r="C39" t="s">
-        <v>644</v>
+        <v>867</v>
       </c>
       <c r="D39" t="s">
-        <v>621</v>
+        <v>868</v>
       </c>
       <c r="AP39" t="s">
-        <v>959</v>
+        <v>391</v>
       </c>
       <c r="BQ39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="CP39" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="40" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>852</v>
+        <v>618</v>
       </c>
       <c r="B40" t="s">
-        <v>863</v>
+        <v>643</v>
       </c>
       <c r="C40" t="s">
-        <v>864</v>
+        <v>644</v>
       </c>
       <c r="D40" t="s">
-        <v>865</v>
+        <v>621</v>
       </c>
       <c r="AP40" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="BQ40" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="CP40" t="s">
-        <v>545</v>
+        <v>593</v>
       </c>
     </row>
     <row r="41" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>673</v>
+        <v>852</v>
       </c>
       <c r="B41" t="s">
-        <v>676</v>
+        <v>863</v>
       </c>
       <c r="C41" t="s">
-        <v>677</v>
+        <v>864</v>
       </c>
       <c r="D41" t="s">
-        <v>738</v>
+        <v>865</v>
+      </c>
+      <c r="AP41" t="s">
+        <v>959</v>
       </c>
       <c r="BQ41" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="CP41" t="s">
-        <v>594</v>
+        <v>545</v>
       </c>
     </row>
     <row r="42" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>618</v>
+        <v>673</v>
       </c>
       <c r="B42" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
       <c r="C42" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
       <c r="D42" t="s">
-        <v>621</v>
+        <v>738</v>
       </c>
       <c r="BQ42" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="CP42" t="s">
-        <v>546</v>
+        <v>594</v>
       </c>
     </row>
     <row r="43" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>750</v>
+        <v>618</v>
       </c>
       <c r="B43" t="s">
-        <v>765</v>
+        <v>649</v>
       </c>
       <c r="C43" t="s">
-        <v>766</v>
+        <v>650</v>
       </c>
       <c r="D43" t="s">
-        <v>753</v>
+        <v>621</v>
       </c>
       <c r="BQ43" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="CP43" t="s">
-        <v>597</v>
+        <v>546</v>
       </c>
     </row>
     <row r="44" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>666</v>
+        <v>750</v>
       </c>
       <c r="B44" t="s">
-        <v>667</v>
+        <v>765</v>
       </c>
       <c r="C44" t="s">
-        <v>668</v>
+        <v>766</v>
       </c>
       <c r="D44" t="s">
-        <v>621</v>
+        <v>753</v>
       </c>
       <c r="BQ44" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="CP44" t="s">
-        <v>715</v>
+        <v>597</v>
       </c>
     </row>
     <row r="45" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="B45" t="s">
-        <v>682</v>
+        <v>667</v>
       </c>
       <c r="C45" t="s">
-        <v>683</v>
+        <v>668</v>
       </c>
       <c r="D45" t="s">
         <v>621</v>
       </c>
       <c r="BQ45" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="CP45" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="46" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>801</v>
+        <v>673</v>
       </c>
       <c r="B46" t="s">
-        <v>816</v>
+        <v>682</v>
       </c>
       <c r="C46" t="s">
-        <v>817</v>
+        <v>683</v>
       </c>
       <c r="D46" t="s">
-        <v>818</v>
+        <v>621</v>
       </c>
       <c r="BQ46" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="CP46" t="s">
-        <v>557</v>
+        <v>716</v>
       </c>
     </row>
     <row r="47" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>719</v>
+        <v>801</v>
       </c>
       <c r="B47" t="s">
-        <v>741</v>
+        <v>816</v>
       </c>
       <c r="C47" t="s">
-        <v>742</v>
+        <v>817</v>
       </c>
       <c r="D47" t="s">
-        <v>729</v>
+        <v>818</v>
       </c>
       <c r="BQ47" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="CP47" t="s">
-        <v>596</v>
+        <v>557</v>
       </c>
     </row>
     <row r="48" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
+        <v>719</v>
+      </c>
+      <c r="B48" t="s">
+        <v>741</v>
+      </c>
+      <c r="C48" t="s">
+        <v>742</v>
+      </c>
+      <c r="D48" t="s">
+        <v>729</v>
+      </c>
+      <c r="BQ48" t="s">
+        <v>487</v>
+      </c>
+      <c r="CP48" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="49" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
         <v>801</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>808</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>809</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>811</v>
       </c>
-      <c r="BQ48" t="s">
+      <c r="BQ49" t="s">
         <v>488</v>
       </c>
-      <c r="CP48" t="s">
+      <c r="CP49" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
+    <row r="50" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>750</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>786</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>787</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
+    <row r="51" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
         <v>618</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>653</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>654</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
+    <row r="52" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
         <v>880</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>896</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>897</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>898</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
+    <row r="53" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
         <v>30</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>28</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>29</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
+    <row r="54" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
         <v>719</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>732</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>733</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
+    <row r="55" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
         <v>852</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>869</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>870</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
+    <row r="56" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
         <v>880</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>881</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>882</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
+    <row r="57" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
         <v>673</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>692</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>693</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
+    <row r="58" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
         <v>880</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>943</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>944</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
+    <row r="59" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>801</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>819</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>820</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>11</v>
-      </c>
-      <c r="B59" t="s">
-        <v>289</v>
-      </c>
-      <c r="C59" t="s">
-        <v>290</v>
-      </c>
-      <c r="D59" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" t="s">
+        <v>289</v>
+      </c>
+      <c r="C60" t="s">
+        <v>290</v>
+      </c>
+      <c r="D60" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="61" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" t="s">
         <v>12</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>13</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
+    <row r="62" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>618</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>645</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>646</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
+    <row r="63" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
         <v>601</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>602</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>603</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
+    <row r="64" spans="1:94" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
         <v>719</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>734</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>735</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>722</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>282</v>
-      </c>
-      <c r="B64" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" t="s">
-        <v>131</v>
-      </c>
-      <c r="D64" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>822</v>
+        <v>282</v>
       </c>
       <c r="B65" t="s">
-        <v>825</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>826</v>
+        <v>131</v>
       </c>
       <c r="D65" t="s">
-        <v>978</v>
+        <v>294</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>750</v>
+        <v>822</v>
       </c>
       <c r="B66" t="s">
-        <v>751</v>
+        <v>825</v>
       </c>
       <c r="C66" t="s">
-        <v>752</v>
+        <v>826</v>
       </c>
       <c r="D66" t="s">
-        <v>754</v>
+        <v>977</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>719</v>
+        <v>750</v>
       </c>
       <c r="B67" t="s">
-        <v>736</v>
+        <v>751</v>
       </c>
       <c r="C67" t="s">
-        <v>737</v>
+        <v>752</v>
       </c>
       <c r="D67" t="s">
-        <v>729</v>
+        <v>754</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>673</v>
+        <v>719</v>
       </c>
       <c r="B68" t="s">
-        <v>680</v>
+        <v>736</v>
       </c>
       <c r="C68" t="s">
-        <v>681</v>
+        <v>737</v>
       </c>
       <c r="D68" t="s">
-        <v>621</v>
+        <v>729</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>30</v>
+        <v>673</v>
       </c>
       <c r="B69" t="s">
-        <v>35</v>
+        <v>680</v>
       </c>
       <c r="C69" t="s">
-        <v>36</v>
+        <v>681</v>
       </c>
       <c r="D69" t="s">
-        <v>292</v>
+        <v>621</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.4">
@@ -6215,55 +6253,55 @@
         <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C70" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D70" t="s">
-        <v>768</v>
+        <v>292</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>822</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>823</v>
+        <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>824</v>
+        <v>51</v>
       </c>
       <c r="D71" t="s">
-        <v>827</v>
+        <v>768</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>30</v>
+        <v>822</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>823</v>
       </c>
       <c r="C72" t="s">
-        <v>85</v>
+        <v>824</v>
       </c>
       <c r="D72" t="s">
-        <v>293</v>
+        <v>827</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>673</v>
+        <v>30</v>
       </c>
       <c r="B73" t="s">
-        <v>694</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
-        <v>695</v>
+        <v>85</v>
       </c>
       <c r="D73" t="s">
-        <v>621</v>
+        <v>293</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.4">
@@ -6271,10 +6309,10 @@
         <v>673</v>
       </c>
       <c r="B74" t="s">
-        <v>674</v>
+        <v>694</v>
       </c>
       <c r="C74" t="s">
-        <v>675</v>
+        <v>695</v>
       </c>
       <c r="D74" t="s">
         <v>621</v>
@@ -6282,58 +6320,58 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>750</v>
+        <v>673</v>
       </c>
       <c r="B75" t="s">
-        <v>755</v>
+        <v>674</v>
       </c>
       <c r="C75" t="s">
-        <v>756</v>
+        <v>675</v>
       </c>
       <c r="D75" t="s">
-        <v>753</v>
+        <v>621</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>618</v>
+        <v>750</v>
       </c>
       <c r="B76" t="s">
-        <v>657</v>
+        <v>755</v>
       </c>
       <c r="C76" t="s">
-        <v>658</v>
+        <v>756</v>
       </c>
       <c r="D76" t="s">
-        <v>621</v>
+        <v>753</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>719</v>
+        <v>618</v>
       </c>
       <c r="B77" t="s">
-        <v>727</v>
+        <v>657</v>
       </c>
       <c r="C77" t="s">
-        <v>728</v>
+        <v>658</v>
       </c>
       <c r="D77" t="s">
-        <v>729</v>
+        <v>621</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>618</v>
+        <v>719</v>
       </c>
       <c r="B78" t="s">
-        <v>638</v>
+        <v>727</v>
       </c>
       <c r="C78" t="s">
-        <v>639</v>
+        <v>728</v>
       </c>
       <c r="D78" t="s">
-        <v>621</v>
+        <v>729</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.4">
@@ -6341,13 +6379,13 @@
         <v>618</v>
       </c>
       <c r="B79" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="C79" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="D79" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.4">
@@ -6355,111 +6393,111 @@
         <v>618</v>
       </c>
       <c r="B80" t="s">
-        <v>619</v>
+        <v>632</v>
       </c>
       <c r="C80" t="s">
-        <v>620</v>
+        <v>633</v>
       </c>
       <c r="D80" t="s">
-        <v>621</v>
+        <v>634</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
-        <v>750</v>
+        <v>618</v>
       </c>
       <c r="B81" t="s">
-        <v>774</v>
+        <v>619</v>
       </c>
       <c r="C81" t="s">
-        <v>775</v>
+        <v>620</v>
       </c>
       <c r="D81" t="s">
-        <v>776</v>
+        <v>621</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
-        <v>673</v>
+        <v>750</v>
       </c>
       <c r="B82" t="s">
-        <v>690</v>
+        <v>774</v>
       </c>
       <c r="C82" t="s">
-        <v>691</v>
+        <v>775</v>
       </c>
       <c r="D82" t="s">
-        <v>621</v>
+        <v>776</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
-        <v>750</v>
+        <v>673</v>
       </c>
       <c r="B83" t="s">
-        <v>757</v>
+        <v>690</v>
       </c>
       <c r="C83" t="s">
-        <v>758</v>
+        <v>691</v>
       </c>
       <c r="D83" t="s">
-        <v>759</v>
+        <v>621</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
-        <v>673</v>
+        <v>750</v>
       </c>
       <c r="B84" t="s">
-        <v>686</v>
+        <v>757</v>
       </c>
       <c r="C84" t="s">
-        <v>687</v>
+        <v>758</v>
       </c>
       <c r="D84" t="s">
-        <v>847</v>
+        <v>759</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
-        <v>822</v>
+        <v>673</v>
       </c>
       <c r="B85" t="s">
-        <v>829</v>
+        <v>686</v>
       </c>
       <c r="C85" t="s">
-        <v>830</v>
+        <v>687</v>
       </c>
       <c r="D85" t="s">
-        <v>831</v>
+        <v>847</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
-        <v>750</v>
+        <v>822</v>
       </c>
       <c r="B86" t="s">
-        <v>777</v>
+        <v>829</v>
       </c>
       <c r="C86" t="s">
-        <v>778</v>
+        <v>830</v>
       </c>
       <c r="D86" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
-        <v>822</v>
+        <v>750</v>
       </c>
       <c r="B87" t="s">
-        <v>844</v>
+        <v>777</v>
       </c>
       <c r="C87" t="s">
-        <v>845</v>
+        <v>778</v>
       </c>
       <c r="D87" t="s">
-        <v>846</v>
+        <v>779</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.4">
@@ -6467,13 +6505,13 @@
         <v>822</v>
       </c>
       <c r="B88" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="C88" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="D88" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.4">
@@ -6481,111 +6519,111 @@
         <v>822</v>
       </c>
       <c r="B89" t="s">
-        <v>836</v>
+        <v>848</v>
       </c>
       <c r="C89" t="s">
-        <v>837</v>
+        <v>849</v>
       </c>
       <c r="D89" t="s">
-        <v>828</v>
+        <v>850</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
-        <v>673</v>
+        <v>822</v>
       </c>
       <c r="B90" t="s">
-        <v>696</v>
+        <v>836</v>
       </c>
       <c r="C90" t="s">
-        <v>697</v>
+        <v>837</v>
       </c>
       <c r="D90" t="s">
-        <v>621</v>
+        <v>828</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
-        <v>801</v>
+        <v>673</v>
       </c>
       <c r="B91" t="s">
-        <v>802</v>
+        <v>696</v>
       </c>
       <c r="C91" t="s">
-        <v>803</v>
+        <v>697</v>
       </c>
       <c r="D91" t="s">
-        <v>810</v>
+        <v>621</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
-        <v>719</v>
+        <v>801</v>
       </c>
       <c r="B92" t="s">
-        <v>739</v>
+        <v>802</v>
       </c>
       <c r="C92" t="s">
-        <v>740</v>
+        <v>803</v>
       </c>
       <c r="D92" t="s">
-        <v>729</v>
+        <v>810</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
-        <v>822</v>
+        <v>719</v>
       </c>
       <c r="B93" t="s">
-        <v>838</v>
+        <v>739</v>
       </c>
       <c r="C93" t="s">
-        <v>839</v>
+        <v>740</v>
       </c>
       <c r="D93" t="s">
-        <v>840</v>
+        <v>729</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>852</v>
+        <v>822</v>
       </c>
       <c r="B94" t="s">
-        <v>853</v>
+        <v>838</v>
       </c>
       <c r="C94" t="s">
-        <v>854</v>
+        <v>839</v>
       </c>
       <c r="D94" t="s">
-        <v>855</v>
+        <v>840</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
-        <v>719</v>
+        <v>852</v>
       </c>
       <c r="B95" t="s">
-        <v>730</v>
+        <v>853</v>
       </c>
       <c r="C95" t="s">
-        <v>731</v>
+        <v>854</v>
       </c>
       <c r="D95" t="s">
-        <v>729</v>
+        <v>855</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
-        <v>618</v>
+        <v>719</v>
       </c>
       <c r="B96" t="s">
-        <v>655</v>
+        <v>730</v>
       </c>
       <c r="C96" t="s">
-        <v>656</v>
+        <v>731</v>
       </c>
       <c r="D96" t="s">
-        <v>621</v>
+        <v>729</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.4">
@@ -6593,27 +6631,27 @@
         <v>618</v>
       </c>
       <c r="B97" t="s">
-        <v>635</v>
+        <v>655</v>
       </c>
       <c r="C97" t="s">
-        <v>636</v>
+        <v>656</v>
       </c>
       <c r="D97" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
-        <v>880</v>
+        <v>618</v>
       </c>
       <c r="B98" t="s">
-        <v>940</v>
+        <v>635</v>
       </c>
       <c r="C98" t="s">
-        <v>941</v>
+        <v>636</v>
       </c>
       <c r="D98" t="s">
-        <v>942</v>
+        <v>637</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.4">
@@ -6621,38 +6659,38 @@
         <v>880</v>
       </c>
       <c r="B99" t="s">
-        <v>884</v>
+        <v>940</v>
       </c>
       <c r="C99" t="s">
-        <v>885</v>
+        <v>941</v>
       </c>
       <c r="D99" t="s">
-        <v>886</v>
+        <v>942</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
-        <v>609</v>
+        <v>880</v>
       </c>
       <c r="B100" t="s">
-        <v>651</v>
+        <v>884</v>
       </c>
       <c r="C100" t="s">
-        <v>652</v>
+        <v>885</v>
+      </c>
+      <c r="D100" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
-        <v>769</v>
+        <v>609</v>
       </c>
       <c r="B101" t="s">
-        <v>784</v>
+        <v>651</v>
       </c>
       <c r="C101" t="s">
-        <v>785</v>
-      </c>
-      <c r="D101" t="s">
-        <v>772</v>
+        <v>652</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.4">
@@ -6660,10 +6698,10 @@
         <v>769</v>
       </c>
       <c r="B102" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="C102" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="D102" t="s">
         <v>772</v>
@@ -6671,16 +6709,16 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
-        <v>511</v>
+        <v>769</v>
       </c>
       <c r="B103" t="s">
-        <v>573</v>
+        <v>780</v>
       </c>
       <c r="C103" t="s">
-        <v>562</v>
+        <v>781</v>
       </c>
       <c r="D103" t="s">
-        <v>577</v>
+        <v>772</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.4">
@@ -6688,10 +6726,10 @@
         <v>511</v>
       </c>
       <c r="B104" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C104" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D104" t="s">
         <v>577</v>
@@ -6699,152 +6737,152 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
-        <v>26</v>
+        <v>511</v>
       </c>
       <c r="B105" t="s">
-        <v>62</v>
+        <v>572</v>
       </c>
       <c r="C105" t="s">
-        <v>63</v>
+        <v>563</v>
+      </c>
+      <c r="D105" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
-        <v>511</v>
+        <v>26</v>
       </c>
       <c r="B106" t="s">
-        <v>568</v>
+        <v>62</v>
       </c>
       <c r="C106" t="s">
-        <v>569</v>
+        <v>63</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
-        <v>26</v>
+        <v>511</v>
       </c>
       <c r="B107" t="s">
-        <v>77</v>
+        <v>568</v>
       </c>
       <c r="C107" t="s">
-        <v>27</v>
+        <v>569</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
-        <v>26</v>
+        <v>985</v>
       </c>
       <c r="B108" t="s">
-        <v>64</v>
+        <v>989</v>
       </c>
       <c r="C108" t="s">
-        <v>64</v>
+        <v>990</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
-        <v>511</v>
+        <v>26</v>
       </c>
       <c r="B109" t="s">
-        <v>566</v>
+        <v>77</v>
       </c>
       <c r="C109" t="s">
-        <v>567</v>
-      </c>
-      <c r="D109" t="s">
-        <v>576</v>
+        <v>27</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
-        <v>361</v>
+        <v>26</v>
       </c>
       <c r="B110" t="s">
-        <v>362</v>
+        <v>64</v>
       </c>
       <c r="C110" t="s">
-        <v>363</v>
+        <v>64</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
-        <v>743</v>
+        <v>511</v>
       </c>
       <c r="B111" t="s">
-        <v>744</v>
+        <v>566</v>
       </c>
       <c r="C111" t="s">
-        <v>745</v>
+        <v>567</v>
       </c>
       <c r="D111" t="s">
-        <v>746</v>
+        <v>576</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
-        <v>4</v>
+        <v>361</v>
       </c>
       <c r="B112" t="s">
-        <v>75</v>
+        <v>362</v>
       </c>
       <c r="C112" t="s">
-        <v>10</v>
-      </c>
-      <c r="D112" t="s">
-        <v>612</v>
+        <v>363</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
-        <v>609</v>
+        <v>743</v>
       </c>
       <c r="B113" t="s">
-        <v>610</v>
+        <v>744</v>
       </c>
       <c r="C113" t="s">
-        <v>611</v>
+        <v>745</v>
       </c>
       <c r="D113" t="s">
-        <v>612</v>
+        <v>746</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
-        <v>769</v>
+        <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>770</v>
+        <v>75</v>
       </c>
       <c r="C114" t="s">
-        <v>771</v>
+        <v>10</v>
       </c>
       <c r="D114" t="s">
-        <v>772</v>
+        <v>612</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
-        <v>511</v>
+        <v>609</v>
       </c>
       <c r="B115" t="s">
-        <v>574</v>
+        <v>610</v>
       </c>
       <c r="C115" t="s">
-        <v>512</v>
+        <v>611</v>
+      </c>
+      <c r="D115" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
-        <v>511</v>
+        <v>769</v>
       </c>
       <c r="B116" t="s">
-        <v>575</v>
+        <v>770</v>
       </c>
       <c r="C116" t="s">
-        <v>513</v>
+        <v>771</v>
       </c>
       <c r="D116" t="s">
-        <v>514</v>
+        <v>772</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.4">
@@ -6852,63 +6890,66 @@
         <v>511</v>
       </c>
       <c r="B117" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C117" t="s">
-        <v>579</v>
-      </c>
-      <c r="D117" t="s">
-        <v>583</v>
+        <v>512</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
-        <v>4</v>
+        <v>511</v>
       </c>
       <c r="B118" t="s">
-        <v>76</v>
+        <v>575</v>
       </c>
       <c r="C118" t="s">
-        <v>608</v>
+        <v>513</v>
       </c>
       <c r="D118" t="s">
-        <v>612</v>
+        <v>514</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
-        <v>876</v>
+        <v>511</v>
       </c>
       <c r="B119" t="s">
-        <v>877</v>
+        <v>578</v>
       </c>
       <c r="C119" t="s">
-        <v>878</v>
+        <v>579</v>
       </c>
       <c r="D119" t="s">
-        <v>879</v>
+        <v>583</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
-        <v>511</v>
+        <v>4</v>
       </c>
       <c r="B120" t="s">
-        <v>599</v>
+        <v>76</v>
       </c>
       <c r="C120" t="s">
-        <v>600</v>
+        <v>608</v>
+      </c>
+      <c r="D120" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
-        <v>26</v>
+        <v>876</v>
       </c>
       <c r="B121" t="s">
-        <v>97</v>
+        <v>877</v>
       </c>
       <c r="C121" t="s">
-        <v>98</v>
+        <v>878</v>
+      </c>
+      <c r="D121" t="s">
+        <v>879</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.4">
@@ -6916,144 +6957,138 @@
         <v>511</v>
       </c>
       <c r="B122" t="s">
-        <v>571</v>
+        <v>599</v>
       </c>
       <c r="C122" t="s">
-        <v>570</v>
-      </c>
-      <c r="D122" t="s">
-        <v>576</v>
+        <v>600</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
-        <v>511</v>
+        <v>26</v>
       </c>
       <c r="B123" t="s">
-        <v>564</v>
+        <v>97</v>
       </c>
       <c r="C123" t="s">
-        <v>565</v>
-      </c>
-      <c r="D123" t="s">
-        <v>576</v>
+        <v>98</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
-        <v>26</v>
+        <v>511</v>
       </c>
       <c r="B124" t="s">
-        <v>33</v>
+        <v>571</v>
       </c>
       <c r="C124" t="s">
-        <v>34</v>
+        <v>570</v>
+      </c>
+      <c r="D124" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
-        <v>26</v>
+        <v>511</v>
       </c>
       <c r="B125" t="s">
-        <v>31</v>
+        <v>564</v>
       </c>
       <c r="C125" t="s">
-        <v>32</v>
+        <v>565</v>
+      </c>
+      <c r="D125" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
-        <v>511</v>
+        <v>26</v>
       </c>
       <c r="B126" t="s">
-        <v>589</v>
+        <v>33</v>
       </c>
       <c r="C126" t="s">
-        <v>590</v>
-      </c>
-      <c r="D126" t="s">
-        <v>591</v>
+        <v>34</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
-        <v>286</v>
+        <v>26</v>
       </c>
       <c r="B127" t="s">
-        <v>287</v>
+        <v>31</v>
       </c>
       <c r="C127" t="s">
-        <v>288</v>
+        <v>32</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
-        <v>4</v>
+        <v>511</v>
       </c>
       <c r="B128" t="s">
-        <v>78</v>
+        <v>589</v>
       </c>
       <c r="C128" t="s">
-        <v>9</v>
+        <v>590</v>
       </c>
       <c r="D128" t="s">
-        <v>612</v>
+        <v>591</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
-        <v>4</v>
+        <v>286</v>
       </c>
       <c r="B129" t="s">
-        <v>79</v>
+        <v>287</v>
       </c>
       <c r="C129" t="s">
-        <v>7</v>
-      </c>
-      <c r="D129" t="s">
-        <v>612</v>
+        <v>288</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
-        <v>769</v>
+        <v>4</v>
       </c>
       <c r="B130" t="s">
-        <v>782</v>
+        <v>78</v>
       </c>
       <c r="C130" t="s">
-        <v>783</v>
+        <v>9</v>
       </c>
       <c r="D130" t="s">
-        <v>772</v>
+        <v>612</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
-        <v>511</v>
+        <v>4</v>
       </c>
       <c r="B131" t="s">
-        <v>584</v>
+        <v>79</v>
       </c>
       <c r="C131" t="s">
-        <v>585</v>
+        <v>7</v>
       </c>
       <c r="D131" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
-        <v>511</v>
+        <v>769</v>
       </c>
       <c r="B132" t="s">
-        <v>580</v>
+        <v>782</v>
       </c>
       <c r="C132" t="s">
-        <v>581</v>
+        <v>783</v>
       </c>
       <c r="D132" t="s">
-        <v>582</v>
+        <v>772</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.4">
@@ -7061,105 +7096,105 @@
         <v>511</v>
       </c>
       <c r="B133" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C133" t="s">
-        <v>587</v>
+        <v>585</v>
+      </c>
+      <c r="D133" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
-        <v>4</v>
+        <v>511</v>
       </c>
       <c r="B134" t="s">
-        <v>80</v>
+        <v>580</v>
       </c>
       <c r="C134" t="s">
-        <v>8</v>
+        <v>581</v>
       </c>
       <c r="D134" t="s">
-        <v>612</v>
+        <v>582</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
-        <v>26</v>
+        <v>511</v>
       </c>
       <c r="B135" t="s">
-        <v>60</v>
+        <v>586</v>
       </c>
       <c r="C135" t="s">
-        <v>61</v>
+        <v>587</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
-        <v>4</v>
+        <v>985</v>
       </c>
       <c r="B136" t="s">
-        <v>81</v>
+        <v>986</v>
       </c>
       <c r="C136" t="s">
-        <v>6</v>
+        <v>987</v>
       </c>
       <c r="D136" t="s">
-        <v>612</v>
+        <v>988</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
-        <v>872</v>
+        <v>4</v>
       </c>
       <c r="B137" t="s">
-        <v>930</v>
+        <v>80</v>
       </c>
       <c r="C137" t="s">
-        <v>931</v>
+        <v>8</v>
       </c>
       <c r="D137" t="s">
-        <v>904</v>
+        <v>612</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
-        <v>872</v>
+        <v>26</v>
       </c>
       <c r="B138" t="s">
-        <v>887</v>
+        <v>60</v>
       </c>
       <c r="C138" t="s">
-        <v>888</v>
-      </c>
-      <c r="D138" t="s">
-        <v>906</v>
+        <v>61</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B139" t="s">
-        <v>671</v>
+        <v>81</v>
       </c>
       <c r="C139" t="s">
-        <v>954</v>
+        <v>6</v>
       </c>
       <c r="D139" t="s">
-        <v>672</v>
+        <v>612</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
-        <v>67</v>
+        <v>872</v>
       </c>
       <c r="B140" t="s">
-        <v>616</v>
+        <v>930</v>
       </c>
       <c r="C140" t="s">
-        <v>617</v>
+        <v>931</v>
       </c>
       <c r="D140" t="s">
-        <v>929</v>
+        <v>904</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.4">
@@ -7167,97 +7202,97 @@
         <v>872</v>
       </c>
       <c r="B141" t="s">
-        <v>902</v>
+        <v>887</v>
       </c>
       <c r="C141" t="s">
-        <v>903</v>
+        <v>888</v>
       </c>
       <c r="D141" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
-        <v>698</v>
+        <v>67</v>
       </c>
       <c r="B142" t="s">
-        <v>712</v>
+        <v>671</v>
       </c>
       <c r="C142" t="s">
-        <v>713</v>
+        <v>954</v>
       </c>
       <c r="D142" t="s">
-        <v>714</v>
+        <v>672</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
-        <v>698</v>
+        <v>67</v>
       </c>
       <c r="B143" t="s">
-        <v>709</v>
+        <v>616</v>
       </c>
       <c r="C143" t="s">
-        <v>710</v>
+        <v>617</v>
       </c>
       <c r="D143" t="s">
-        <v>711</v>
+        <v>929</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
-        <v>67</v>
+        <v>872</v>
       </c>
       <c r="B144" t="s">
-        <v>68</v>
+        <v>902</v>
       </c>
       <c r="C144" t="s">
-        <v>895</v>
+        <v>903</v>
       </c>
       <c r="D144" t="s">
-        <v>89</v>
+        <v>904</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
-        <v>872</v>
+        <v>698</v>
       </c>
       <c r="B145" t="s">
-        <v>917</v>
+        <v>712</v>
       </c>
       <c r="C145" t="s">
-        <v>918</v>
+        <v>713</v>
       </c>
       <c r="D145" t="s">
-        <v>919</v>
+        <v>714</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
-        <v>872</v>
+        <v>698</v>
       </c>
       <c r="B146" t="s">
-        <v>873</v>
+        <v>709</v>
       </c>
       <c r="C146" t="s">
-        <v>874</v>
+        <v>710</v>
       </c>
       <c r="D146" t="s">
-        <v>875</v>
+        <v>711</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
-        <v>698</v>
+        <v>67</v>
       </c>
       <c r="B147" t="s">
-        <v>699</v>
+        <v>68</v>
       </c>
       <c r="C147" t="s">
-        <v>851</v>
+        <v>895</v>
       </c>
       <c r="D147" t="s">
-        <v>700</v>
+        <v>89</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.4">
@@ -7265,66 +7300,66 @@
         <v>872</v>
       </c>
       <c r="B148" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="C148" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="D148" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
-        <v>760</v>
+        <v>872</v>
       </c>
       <c r="B149" t="s">
-        <v>763</v>
+        <v>873</v>
       </c>
       <c r="C149" t="s">
-        <v>764</v>
+        <v>874</v>
       </c>
       <c r="D149" t="s">
-        <v>90</v>
+        <v>875</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
-        <v>613</v>
+        <v>698</v>
       </c>
       <c r="B150" t="s">
-        <v>640</v>
+        <v>699</v>
       </c>
       <c r="C150" t="s">
-        <v>641</v>
+        <v>851</v>
       </c>
       <c r="D150" t="s">
-        <v>642</v>
+        <v>700</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
-        <v>613</v>
+        <v>872</v>
       </c>
       <c r="B151" t="s">
-        <v>622</v>
+        <v>920</v>
       </c>
       <c r="C151" t="s">
-        <v>623</v>
+        <v>921</v>
       </c>
       <c r="D151" t="s">
-        <v>624</v>
+        <v>922</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
-        <v>605</v>
+        <v>760</v>
       </c>
       <c r="B152" t="s">
-        <v>606</v>
+        <v>763</v>
       </c>
       <c r="C152" t="s">
-        <v>625</v>
+        <v>764</v>
       </c>
       <c r="D152" t="s">
         <v>90</v>
@@ -7332,58 +7367,58 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
-        <v>67</v>
+        <v>613</v>
       </c>
       <c r="B153" t="s">
-        <v>88</v>
+        <v>640</v>
       </c>
       <c r="C153" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
       <c r="D153" t="s">
-        <v>90</v>
+        <v>642</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
-        <v>872</v>
+        <v>613</v>
       </c>
       <c r="B154" t="s">
-        <v>910</v>
+        <v>622</v>
       </c>
       <c r="C154" t="s">
-        <v>911</v>
+        <v>623</v>
       </c>
       <c r="D154" t="s">
-        <v>912</v>
+        <v>624</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
-        <v>698</v>
+        <v>605</v>
       </c>
       <c r="B155" t="s">
-        <v>707</v>
+        <v>606</v>
       </c>
       <c r="C155" t="s">
-        <v>708</v>
+        <v>625</v>
       </c>
       <c r="D155" t="s">
-        <v>916</v>
+        <v>90</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
-        <v>698</v>
+        <v>67</v>
       </c>
       <c r="B156" t="s">
-        <v>703</v>
+        <v>88</v>
       </c>
       <c r="C156" t="s">
-        <v>704</v>
+        <v>626</v>
       </c>
       <c r="D156" t="s">
-        <v>705</v>
+        <v>90</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.4">
@@ -7391,13 +7426,13 @@
         <v>872</v>
       </c>
       <c r="B157" t="s">
-        <v>889</v>
+        <v>910</v>
       </c>
       <c r="C157" t="s">
-        <v>890</v>
+        <v>911</v>
       </c>
       <c r="D157" t="s">
-        <v>905</v>
+        <v>912</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.4">
@@ -7405,27 +7440,27 @@
         <v>698</v>
       </c>
       <c r="B158" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="C158" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="D158" t="s">
-        <v>706</v>
+        <v>916</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
-        <v>872</v>
+        <v>698</v>
       </c>
       <c r="B159" t="s">
-        <v>927</v>
+        <v>703</v>
       </c>
       <c r="C159" t="s">
-        <v>926</v>
+        <v>704</v>
       </c>
       <c r="D159" t="s">
-        <v>928</v>
+        <v>705</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.4">
@@ -7433,27 +7468,27 @@
         <v>872</v>
       </c>
       <c r="B160" t="s">
-        <v>937</v>
+        <v>889</v>
       </c>
       <c r="C160" t="s">
-        <v>938</v>
+        <v>890</v>
       </c>
       <c r="D160" t="s">
-        <v>939</v>
+        <v>905</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
-        <v>760</v>
+        <v>698</v>
       </c>
       <c r="B161" t="s">
-        <v>761</v>
+        <v>701</v>
       </c>
       <c r="C161" t="s">
-        <v>762</v>
+        <v>702</v>
       </c>
       <c r="D161" t="s">
-        <v>807</v>
+        <v>706</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.4">
@@ -7461,41 +7496,41 @@
         <v>872</v>
       </c>
       <c r="B162" t="s">
-        <v>907</v>
+        <v>927</v>
       </c>
       <c r="C162" t="s">
-        <v>908</v>
+        <v>926</v>
       </c>
       <c r="D162" t="s">
-        <v>909</v>
+        <v>928</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
-        <v>804</v>
+        <v>872</v>
       </c>
       <c r="B163" t="s">
-        <v>805</v>
+        <v>937</v>
       </c>
       <c r="C163" t="s">
-        <v>805</v>
+        <v>938</v>
       </c>
       <c r="D163" t="s">
-        <v>806</v>
+        <v>939</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
-        <v>872</v>
+        <v>760</v>
       </c>
       <c r="B164" t="s">
-        <v>923</v>
+        <v>761</v>
       </c>
       <c r="C164" t="s">
-        <v>924</v>
+        <v>762</v>
       </c>
       <c r="D164" t="s">
-        <v>925</v>
+        <v>807</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.4">
@@ -7503,191 +7538,233 @@
         <v>872</v>
       </c>
       <c r="B165" t="s">
+        <v>907</v>
+      </c>
+      <c r="C165" t="s">
+        <v>908</v>
+      </c>
+      <c r="D165" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A166" t="s">
+        <v>804</v>
+      </c>
+      <c r="B166" t="s">
+        <v>805</v>
+      </c>
+      <c r="C166" t="s">
+        <v>805</v>
+      </c>
+      <c r="D166" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A167" t="s">
+        <v>872</v>
+      </c>
+      <c r="B167" t="s">
+        <v>923</v>
+      </c>
+      <c r="C167" t="s">
+        <v>924</v>
+      </c>
+      <c r="D167" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A168" t="s">
+        <v>872</v>
+      </c>
+      <c r="B168" t="s">
         <v>935</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C168" t="s">
         <v>936</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B166" t="s">
-        <v>515</v>
-      </c>
-      <c r="C166" t="s">
-        <v>41</v>
-      </c>
-      <c r="D166" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B167" t="s">
-        <v>72</v>
-      </c>
-      <c r="C167" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B168" t="s">
-        <v>48</v>
-      </c>
-      <c r="C168" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B169" t="s">
-        <v>55</v>
+        <v>515</v>
       </c>
       <c r="C169" t="s">
-        <v>56</v>
+        <v>41</v>
+      </c>
+      <c r="D169" t="s">
+        <v>718</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B170" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C170" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B171" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C171" t="s">
-        <v>21</v>
-      </c>
-      <c r="D171" t="s">
-        <v>360</v>
+        <v>49</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B172" t="s">
-        <v>664</v>
+        <v>55</v>
       </c>
       <c r="C172" t="s">
-        <v>665</v>
+        <v>56</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B173" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
       <c r="C173" t="s">
-        <v>561</v>
+        <v>91</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B174" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="C174" t="s">
-        <v>284</v>
+        <v>21</v>
+      </c>
+      <c r="D174" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B175" t="s">
-        <v>833</v>
+        <v>664</v>
       </c>
       <c r="C175" t="s">
-        <v>834</v>
+        <v>665</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B176" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="C176" t="s">
-        <v>47</v>
+        <v>561</v>
       </c>
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B177" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="C177" t="s">
-        <v>99</v>
+        <v>284</v>
       </c>
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B178" t="s">
-        <v>22</v>
+        <v>833</v>
       </c>
       <c r="C178" t="s">
-        <v>23</v>
+        <v>834</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B179" t="s">
-        <v>773</v>
+        <v>46</v>
       </c>
       <c r="C179" t="s">
-        <v>835</v>
+        <v>47</v>
       </c>
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B180" t="s">
-        <v>559</v>
+        <v>52</v>
       </c>
       <c r="C180" t="s">
-        <v>560</v>
+        <v>99</v>
       </c>
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B181" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C181" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B182" t="s">
-        <v>82</v>
+        <v>773</v>
       </c>
       <c r="C182" t="s">
-        <v>83</v>
+        <v>835</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B183" t="s">
-        <v>39</v>
+        <v>559</v>
       </c>
       <c r="C183" t="s">
-        <v>40</v>
+        <v>560</v>
       </c>
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B184" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C184" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B185" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="C185" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B186" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C186" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B187" t="s">
+        <v>53</v>
+      </c>
+      <c r="C187" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B188" t="s">
+        <v>37</v>
+      </c>
+      <c r="C188" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B189" t="s">
+        <v>24</v>
+      </c>
+      <c r="C189" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B190" t="s">
         <v>295</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C190" t="s">
         <v>296</v>
       </c>
     </row>
@@ -7705,7 +7782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -7831,7 +7908,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Radio/TV (PAWS), CD/VHS
</commit_message>
<xml_diff>
--- a/프좀 용어집.xlsx
+++ b/프좀 용어집.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947F0006-2F6F-4D4A-863E-B0CEE5BC7901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C29F15F-F83C-4381-A22C-0B13E13E4DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3576" yWindow="696" windowWidth="17280" windowHeight="10728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4364,8 +4364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Update Radio/TV (ect), CD/VHS
ect: Adverts, Civilian Radio, Unknown Frequency
</commit_message>
<xml_diff>
--- a/프좀 용어집.xlsx
+++ b/프좀 용어집.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C29F15F-F83C-4381-A22C-0B13E13E4DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9B569F-2203-4D31-B521-8F962E7D651E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3576" yWindow="696" windowWidth="17280" windowHeight="10728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3576" yWindow="696" windowWidth="17280" windowHeight="10728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="라디오,TV" sheetId="1" r:id="rId1"/>
@@ -2830,10 +2830,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>녹스 히트는 해요체</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>격리 구역(exclusion zone)과 사용되었을 때</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3911,6 +3907,10 @@
   </si>
   <si>
     <t>할리우드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>녹스 히트는 해요체 - X, 합니다로 통일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4364,8 +4364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4392,16 +4392,16 @@
     </row>
     <row r="2" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B2" t="s">
+        <v>912</v>
+      </c>
+      <c r="C2" t="s">
         <v>913</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>914</v>
-      </c>
-      <c r="D2" t="s">
-        <v>915</v>
       </c>
       <c r="F2" t="s">
         <v>128</v>
@@ -4416,7 +4416,7 @@
         <v>298</v>
       </c>
       <c r="AP2" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="AY2" t="s">
         <v>392</v>
@@ -4453,16 +4453,16 @@
     </row>
     <row r="4" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>855</v>
+      </c>
+      <c r="B4" t="s">
         <v>856</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>857</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>858</v>
-      </c>
-      <c r="D4" t="s">
-        <v>859</v>
       </c>
       <c r="F4" t="s">
         <v>114</v>
@@ -4486,7 +4486,7 @@
         <v>418</v>
       </c>
       <c r="BQ4" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="BZ4" t="s">
         <v>517</v>
@@ -4574,7 +4574,7 @@
         <v>420</v>
       </c>
       <c r="BQ6" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="BZ6" t="s">
         <v>519</v>
@@ -4632,16 +4632,16 @@
     </row>
     <row r="8" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
+        <v>722</v>
+      </c>
+      <c r="B8" t="s">
         <v>723</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>724</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>725</v>
-      </c>
-      <c r="D8" t="s">
-        <v>726</v>
       </c>
       <c r="F8" t="s">
         <v>118</v>
@@ -4676,16 +4676,16 @@
     </row>
     <row r="9" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B9" t="s">
+        <v>898</v>
+      </c>
+      <c r="C9" t="s">
         <v>899</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>900</v>
-      </c>
-      <c r="D9" t="s">
-        <v>901</v>
       </c>
       <c r="F9" t="s">
         <v>119</v>
@@ -4723,16 +4723,16 @@
     </row>
     <row r="10" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
+        <v>890</v>
+      </c>
+      <c r="B10" t="s">
         <v>891</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>892</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>893</v>
-      </c>
-      <c r="D10" t="s">
-        <v>894</v>
       </c>
       <c r="F10" t="s">
         <v>120</v>
@@ -4811,16 +4811,16 @@
     </row>
     <row r="12" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B12" t="s">
+        <v>931</v>
+      </c>
+      <c r="C12" t="s">
         <v>932</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>933</v>
-      </c>
-      <c r="D12" t="s">
-        <v>934</v>
       </c>
       <c r="F12" t="s">
         <v>122</v>
@@ -4858,16 +4858,16 @@
     </row>
     <row r="13" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>811</v>
+      </c>
+      <c r="B13" t="s">
         <v>812</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>813</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>814</v>
-      </c>
-      <c r="D13" t="s">
-        <v>815</v>
       </c>
       <c r="F13" t="s">
         <v>123</v>
@@ -4899,16 +4899,16 @@
     </row>
     <row r="14" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B14" t="s">
+        <v>859</v>
+      </c>
+      <c r="C14" t="s">
         <v>860</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>861</v>
-      </c>
-      <c r="D14" t="s">
-        <v>862</v>
       </c>
       <c r="F14" t="s">
         <v>124</v>
@@ -5051,16 +5051,16 @@
     </row>
     <row r="18" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>945</v>
+      </c>
+      <c r="B18" t="s">
         <v>946</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>947</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>948</v>
-      </c>
-      <c r="D18" t="s">
-        <v>949</v>
       </c>
       <c r="N18" t="s">
         <v>343</v>
@@ -5092,16 +5092,16 @@
     </row>
     <row r="19" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B19" t="s">
+        <v>954</v>
+      </c>
+      <c r="C19" t="s">
         <v>955</v>
       </c>
-      <c r="C19" t="s">
-        <v>956</v>
-      </c>
       <c r="D19" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F19" t="s">
         <v>100</v>
@@ -5133,16 +5133,16 @@
     </row>
     <row r="20" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B20" t="s">
+        <v>964</v>
+      </c>
+      <c r="C20" t="s">
         <v>965</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>966</v>
-      </c>
-      <c r="D20" t="s">
-        <v>967</v>
       </c>
       <c r="F20" t="s">
         <v>101</v>
@@ -5177,7 +5177,7 @@
         <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D21" t="s">
         <v>285</v>
@@ -5215,16 +5215,16 @@
     </row>
     <row r="22" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B22" t="s">
+        <v>962</v>
+      </c>
+      <c r="C22" t="s">
         <v>963</v>
       </c>
-      <c r="C22" t="s">
-        <v>964</v>
-      </c>
       <c r="D22" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="AH22" t="s">
         <v>322</v>
@@ -5241,16 +5241,16 @@
     </row>
     <row r="23" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
+        <v>949</v>
+      </c>
+      <c r="B23" t="s">
         <v>950</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>951</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>952</v>
-      </c>
-      <c r="D23" t="s">
-        <v>953</v>
       </c>
       <c r="F23" t="s">
         <v>103</v>
@@ -5285,16 +5285,16 @@
     </row>
     <row r="24" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
+        <v>969</v>
+      </c>
+      <c r="B24" t="s">
+        <v>971</v>
+      </c>
+      <c r="C24" t="s">
         <v>970</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>972</v>
-      </c>
-      <c r="C24" t="s">
-        <v>971</v>
-      </c>
-      <c r="D24" t="s">
-        <v>973</v>
       </c>
       <c r="F24" t="s">
         <v>104</v>
@@ -5303,7 +5303,7 @@
         <v>348</v>
       </c>
       <c r="AH24" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AP24" t="s">
         <v>382</v>
@@ -5326,16 +5326,16 @@
     </row>
     <row r="25" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B25" t="s">
+        <v>973</v>
+      </c>
+      <c r="C25" t="s">
+        <v>975</v>
+      </c>
+      <c r="D25" t="s">
         <v>974</v>
-      </c>
-      <c r="C25" t="s">
-        <v>976</v>
-      </c>
-      <c r="D25" t="s">
-        <v>975</v>
       </c>
       <c r="F25" t="s">
         <v>105</v>
@@ -5367,16 +5367,16 @@
     </row>
     <row r="26" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B26" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C26" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D26" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="AH26" t="s">
         <v>325</v>
@@ -5405,7 +5405,7 @@
         <v>440</v>
       </c>
       <c r="BQ27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="28" spans="1:94" x14ac:dyDescent="0.4">
@@ -5433,16 +5433,16 @@
     </row>
     <row r="29" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
+        <v>979</v>
+      </c>
+      <c r="B29" t="s">
+        <v>981</v>
+      </c>
+      <c r="C29" t="s">
         <v>980</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>982</v>
-      </c>
-      <c r="C29" t="s">
-        <v>981</v>
-      </c>
-      <c r="D29" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="30" spans="1:94" x14ac:dyDescent="0.4">
@@ -5477,7 +5477,7 @@
         <v>442</v>
       </c>
       <c r="BQ30" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="CI30" t="s">
         <v>507</v>
@@ -5488,16 +5488,16 @@
     </row>
     <row r="31" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B31" t="s">
+        <v>746</v>
+      </c>
+      <c r="C31" t="s">
         <v>747</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>748</v>
-      </c>
-      <c r="D31" t="s">
-        <v>749</v>
       </c>
       <c r="F31" t="s">
         <v>107</v>
@@ -5529,16 +5529,16 @@
     </row>
     <row r="32" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
+        <v>718</v>
+      </c>
+      <c r="B32" t="s">
         <v>719</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>720</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>721</v>
-      </c>
-      <c r="D32" t="s">
-        <v>722</v>
       </c>
       <c r="F32" t="s">
         <v>108</v>
@@ -5547,7 +5547,7 @@
         <v>352</v>
       </c>
       <c r="AP32" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="BH32" t="s">
         <v>444</v>
@@ -5741,16 +5741,16 @@
     </row>
     <row r="39" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B39" t="s">
+        <v>865</v>
+      </c>
+      <c r="C39" t="s">
         <v>866</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>867</v>
-      </c>
-      <c r="D39" t="s">
-        <v>868</v>
       </c>
       <c r="AP39" t="s">
         <v>391</v>
@@ -5776,7 +5776,7 @@
         <v>621</v>
       </c>
       <c r="AP40" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="BQ40" t="s">
         <v>479</v>
@@ -5787,19 +5787,19 @@
     </row>
     <row r="41" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B41" t="s">
+        <v>862</v>
+      </c>
+      <c r="C41" t="s">
         <v>863</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>864</v>
       </c>
-      <c r="D41" t="s">
-        <v>865</v>
-      </c>
       <c r="AP41" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="BQ41" t="s">
         <v>481</v>
@@ -5819,7 +5819,7 @@
         <v>677</v>
       </c>
       <c r="D42" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="BQ42" t="s">
         <v>480</v>
@@ -5850,16 +5850,16 @@
     </row>
     <row r="44" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B44" t="s">
+        <v>764</v>
+      </c>
+      <c r="C44" t="s">
         <v>765</v>
       </c>
-      <c r="C44" t="s">
-        <v>766</v>
-      </c>
       <c r="D44" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="BQ44" t="s">
         <v>483</v>
@@ -5910,16 +5910,16 @@
     </row>
     <row r="47" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B47" t="s">
+        <v>815</v>
+      </c>
+      <c r="C47" t="s">
         <v>816</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>817</v>
-      </c>
-      <c r="D47" t="s">
-        <v>818</v>
       </c>
       <c r="BQ47" t="s">
         <v>486</v>
@@ -5930,16 +5930,16 @@
     </row>
     <row r="48" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B48" t="s">
+        <v>740</v>
+      </c>
+      <c r="C48" t="s">
         <v>741</v>
       </c>
-      <c r="C48" t="s">
-        <v>742</v>
-      </c>
       <c r="D48" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="BQ48" t="s">
         <v>487</v>
@@ -5950,16 +5950,16 @@
     </row>
     <row r="49" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B49" t="s">
+        <v>807</v>
+      </c>
+      <c r="C49" t="s">
         <v>808</v>
       </c>
-      <c r="C49" t="s">
-        <v>809</v>
-      </c>
       <c r="D49" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="BQ49" t="s">
         <v>488</v>
@@ -5970,16 +5970,16 @@
     </row>
     <row r="50" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B50" t="s">
+        <v>785</v>
+      </c>
+      <c r="C50" t="s">
         <v>786</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>787</v>
-      </c>
-      <c r="D50" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="51" spans="1:94" x14ac:dyDescent="0.4">
@@ -5998,16 +5998,16 @@
     </row>
     <row r="52" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B52" t="s">
+        <v>895</v>
+      </c>
+      <c r="C52" t="s">
         <v>896</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>897</v>
-      </c>
-      <c r="D52" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="53" spans="1:94" x14ac:dyDescent="0.4">
@@ -6026,44 +6026,44 @@
     </row>
     <row r="54" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B54" t="s">
+        <v>731</v>
+      </c>
+      <c r="C54" t="s">
         <v>732</v>
       </c>
-      <c r="C54" t="s">
-        <v>733</v>
-      </c>
       <c r="D54" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="55" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B55" t="s">
+        <v>868</v>
+      </c>
+      <c r="C55" t="s">
         <v>869</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>870</v>
-      </c>
-      <c r="D55" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="56" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
+        <v>879</v>
+      </c>
+      <c r="B56" t="s">
         <v>880</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>881</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>882</v>
-      </c>
-      <c r="D56" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="57" spans="1:94" x14ac:dyDescent="0.4">
@@ -6082,30 +6082,30 @@
     </row>
     <row r="58" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B58" t="s">
+        <v>942</v>
+      </c>
+      <c r="C58" t="s">
         <v>943</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>944</v>
-      </c>
-      <c r="D58" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="59" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B59" t="s">
+        <v>818</v>
+      </c>
+      <c r="C59" t="s">
         <v>819</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>820</v>
-      </c>
-      <c r="D59" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="60" spans="1:94" x14ac:dyDescent="0.4">
@@ -6119,7 +6119,7 @@
         <v>290</v>
       </c>
       <c r="D60" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="61" spans="1:94" x14ac:dyDescent="0.4">
@@ -6166,16 +6166,16 @@
     </row>
     <row r="64" spans="1:94" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B64" t="s">
+        <v>733</v>
+      </c>
+      <c r="C64" t="s">
         <v>734</v>
       </c>
-      <c r="C64" t="s">
-        <v>735</v>
-      </c>
       <c r="D64" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.4">
@@ -6194,44 +6194,44 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B66" t="s">
+        <v>824</v>
+      </c>
+      <c r="C66" t="s">
         <v>825</v>
       </c>
-      <c r="C66" t="s">
-        <v>826</v>
-      </c>
       <c r="D66" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
+        <v>749</v>
+      </c>
+      <c r="B67" t="s">
         <v>750</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>751</v>
       </c>
-      <c r="C67" t="s">
-        <v>752</v>
-      </c>
       <c r="D67" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B68" t="s">
+        <v>735</v>
+      </c>
+      <c r="C68" t="s">
         <v>736</v>
       </c>
-      <c r="C68" t="s">
-        <v>737</v>
-      </c>
       <c r="D68" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.4">
@@ -6273,21 +6273,21 @@
         <v>51</v>
       </c>
       <c r="D71" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
+        <v>821</v>
+      </c>
+      <c r="B72" t="s">
         <v>822</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>823</v>
       </c>
-      <c r="C72" t="s">
-        <v>824</v>
-      </c>
       <c r="D72" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.4">
@@ -6334,16 +6334,16 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B76" t="s">
+        <v>754</v>
+      </c>
+      <c r="C76" t="s">
         <v>755</v>
       </c>
-      <c r="C76" t="s">
-        <v>756</v>
-      </c>
       <c r="D76" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.4">
@@ -6362,16 +6362,16 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B78" t="s">
+        <v>726</v>
+      </c>
+      <c r="C78" t="s">
         <v>727</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>728</v>
-      </c>
-      <c r="D78" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.4">
@@ -6418,16 +6418,16 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B82" t="s">
+        <v>773</v>
+      </c>
+      <c r="C82" t="s">
         <v>774</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>775</v>
-      </c>
-      <c r="D82" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.4">
@@ -6446,16 +6446,16 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B84" t="s">
+        <v>756</v>
+      </c>
+      <c r="C84" t="s">
         <v>757</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>758</v>
-      </c>
-      <c r="D84" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.4">
@@ -6469,77 +6469,77 @@
         <v>687</v>
       </c>
       <c r="D85" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B86" t="s">
+        <v>828</v>
+      </c>
+      <c r="C86" t="s">
         <v>829</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>830</v>
-      </c>
-      <c r="D86" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B87" t="s">
+        <v>776</v>
+      </c>
+      <c r="C87" t="s">
         <v>777</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>778</v>
-      </c>
-      <c r="D87" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B88" t="s">
+        <v>843</v>
+      </c>
+      <c r="C88" t="s">
         <v>844</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>845</v>
-      </c>
-      <c r="D88" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B89" t="s">
+        <v>847</v>
+      </c>
+      <c r="C89" t="s">
         <v>848</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>849</v>
-      </c>
-      <c r="D89" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B90" t="s">
+        <v>835</v>
+      </c>
+      <c r="C90" t="s">
         <v>836</v>
       </c>
-      <c r="C90" t="s">
-        <v>837</v>
-      </c>
       <c r="D90" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.4">
@@ -6558,72 +6558,72 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
+        <v>800</v>
+      </c>
+      <c r="B92" t="s">
         <v>801</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>802</v>
       </c>
-      <c r="C92" t="s">
-        <v>803</v>
-      </c>
       <c r="D92" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B93" t="s">
+        <v>738</v>
+      </c>
+      <c r="C93" t="s">
         <v>739</v>
       </c>
-      <c r="C93" t="s">
-        <v>740</v>
-      </c>
       <c r="D93" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B94" t="s">
+        <v>837</v>
+      </c>
+      <c r="C94" t="s">
         <v>838</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>839</v>
-      </c>
-      <c r="D94" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
+        <v>851</v>
+      </c>
+      <c r="B95" t="s">
         <v>852</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>853</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>854</v>
-      </c>
-      <c r="D95" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B96" t="s">
+        <v>729</v>
+      </c>
+      <c r="C96" t="s">
         <v>730</v>
       </c>
-      <c r="C96" t="s">
-        <v>731</v>
-      </c>
       <c r="D96" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.4">
@@ -6656,30 +6656,30 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B99" t="s">
+        <v>939</v>
+      </c>
+      <c r="C99" t="s">
         <v>940</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>941</v>
-      </c>
-      <c r="D99" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B100" t="s">
+        <v>883</v>
+      </c>
+      <c r="C100" t="s">
         <v>884</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>885</v>
-      </c>
-      <c r="D100" t="s">
-        <v>886</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.4">
@@ -6695,30 +6695,30 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B102" t="s">
+        <v>783</v>
+      </c>
+      <c r="C102" t="s">
         <v>784</v>
       </c>
-      <c r="C102" t="s">
-        <v>785</v>
-      </c>
       <c r="D102" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B103" t="s">
+        <v>779</v>
+      </c>
+      <c r="C103" t="s">
         <v>780</v>
       </c>
-      <c r="C103" t="s">
-        <v>781</v>
-      </c>
       <c r="D103" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.4">
@@ -6773,13 +6773,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B108" t="s">
+        <v>988</v>
+      </c>
+      <c r="C108" t="s">
         <v>989</v>
-      </c>
-      <c r="C108" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.4">
@@ -6831,16 +6831,16 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
+        <v>742</v>
+      </c>
+      <c r="B113" t="s">
         <v>743</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>744</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="s">
         <v>745</v>
-      </c>
-      <c r="D113" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.4">
@@ -6873,16 +6873,16 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
+        <v>768</v>
+      </c>
+      <c r="B116" t="s">
         <v>769</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>770</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>771</v>
-      </c>
-      <c r="D116" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.4">
@@ -6940,16 +6940,16 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
+        <v>875</v>
+      </c>
+      <c r="B121" t="s">
         <v>876</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>877</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
         <v>878</v>
-      </c>
-      <c r="D121" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.4">
@@ -7079,16 +7079,16 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B132" t="s">
+        <v>781</v>
+      </c>
+      <c r="C132" t="s">
         <v>782</v>
       </c>
-      <c r="C132" t="s">
-        <v>783</v>
-      </c>
       <c r="D132" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.4">
@@ -7132,16 +7132,16 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
+        <v>984</v>
+      </c>
+      <c r="B136" t="s">
         <v>985</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
         <v>986</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D136" t="s">
         <v>987</v>
-      </c>
-      <c r="D136" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.4">
@@ -7185,30 +7185,30 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B140" t="s">
+        <v>929</v>
+      </c>
+      <c r="C140" t="s">
         <v>930</v>
       </c>
-      <c r="C140" t="s">
-        <v>931</v>
-      </c>
       <c r="D140" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B141" t="s">
+        <v>886</v>
+      </c>
+      <c r="C141" t="s">
         <v>887</v>
       </c>
-      <c r="C141" t="s">
-        <v>888</v>
-      </c>
       <c r="D141" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.4">
@@ -7219,7 +7219,7 @@
         <v>671</v>
       </c>
       <c r="C142" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D142" t="s">
         <v>672</v>
@@ -7236,21 +7236,21 @@
         <v>617</v>
       </c>
       <c r="D143" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B144" t="s">
+        <v>901</v>
+      </c>
+      <c r="C144" t="s">
         <v>902</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>903</v>
-      </c>
-      <c r="D144" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.4">
@@ -7289,7 +7289,7 @@
         <v>68</v>
       </c>
       <c r="C147" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D147" t="s">
         <v>89</v>
@@ -7297,30 +7297,30 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B148" t="s">
+        <v>916</v>
+      </c>
+      <c r="C148" t="s">
         <v>917</v>
       </c>
-      <c r="C148" t="s">
+      <c r="D148" t="s">
         <v>918</v>
-      </c>
-      <c r="D148" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
+        <v>871</v>
+      </c>
+      <c r="B149" t="s">
         <v>872</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" t="s">
         <v>873</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
         <v>874</v>
-      </c>
-      <c r="D149" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.4">
@@ -7331,7 +7331,7 @@
         <v>699</v>
       </c>
       <c r="C150" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D150" t="s">
         <v>700</v>
@@ -7339,27 +7339,27 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B151" t="s">
+        <v>919</v>
+      </c>
+      <c r="C151" t="s">
         <v>920</v>
       </c>
-      <c r="C151" t="s">
+      <c r="D151" t="s">
         <v>921</v>
-      </c>
-      <c r="D151" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B152" t="s">
+        <v>762</v>
+      </c>
+      <c r="C152" t="s">
         <v>763</v>
-      </c>
-      <c r="C152" t="s">
-        <v>764</v>
       </c>
       <c r="D152" t="s">
         <v>90</v>
@@ -7423,16 +7423,16 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B157" t="s">
+        <v>909</v>
+      </c>
+      <c r="C157" t="s">
         <v>910</v>
       </c>
-      <c r="C157" t="s">
+      <c r="D157" t="s">
         <v>911</v>
-      </c>
-      <c r="D157" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.4">
@@ -7446,7 +7446,7 @@
         <v>708</v>
       </c>
       <c r="D158" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.4">
@@ -7465,16 +7465,16 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B160" t="s">
+        <v>888</v>
+      </c>
+      <c r="C160" t="s">
         <v>889</v>
       </c>
-      <c r="C160" t="s">
-        <v>890</v>
-      </c>
       <c r="D160" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.4">
@@ -7493,97 +7493,97 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B162" t="s">
+        <v>926</v>
+      </c>
+      <c r="C162" t="s">
+        <v>925</v>
+      </c>
+      <c r="D162" t="s">
         <v>927</v>
-      </c>
-      <c r="C162" t="s">
-        <v>926</v>
-      </c>
-      <c r="D162" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B163" t="s">
+        <v>936</v>
+      </c>
+      <c r="C163" t="s">
         <v>937</v>
       </c>
-      <c r="C163" t="s">
+      <c r="D163" t="s">
         <v>938</v>
-      </c>
-      <c r="D163" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
+        <v>759</v>
+      </c>
+      <c r="B164" t="s">
         <v>760</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" t="s">
         <v>761</v>
       </c>
-      <c r="C164" t="s">
-        <v>762</v>
-      </c>
       <c r="D164" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B165" t="s">
+        <v>906</v>
+      </c>
+      <c r="C165" t="s">
         <v>907</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D165" t="s">
         <v>908</v>
-      </c>
-      <c r="D165" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
+        <v>803</v>
+      </c>
+      <c r="B166" t="s">
         <v>804</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C166" t="s">
+        <v>804</v>
+      </c>
+      <c r="D166" t="s">
         <v>805</v>
-      </c>
-      <c r="C166" t="s">
-        <v>805</v>
-      </c>
-      <c r="D166" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B167" t="s">
+        <v>922</v>
+      </c>
+      <c r="C167" t="s">
         <v>923</v>
       </c>
-      <c r="C167" t="s">
+      <c r="D167" t="s">
         <v>924</v>
-      </c>
-      <c r="D167" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B168" t="s">
+        <v>934</v>
+      </c>
+      <c r="C168" t="s">
         <v>935</v>
-      </c>
-      <c r="C168" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.4">
@@ -7594,7 +7594,7 @@
         <v>41</v>
       </c>
       <c r="D169" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.4">
@@ -7666,10 +7666,10 @@
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B178" t="s">
+        <v>832</v>
+      </c>
+      <c r="C178" t="s">
         <v>833</v>
-      </c>
-      <c r="C178" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.4">
@@ -7698,10 +7698,10 @@
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B182" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C182" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.4">
@@ -7782,8 +7782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -7793,15 +7793,15 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
@@ -7809,10 +7809,10 @@
         <v>535</v>
       </c>
       <c r="G3" t="s">
+        <v>794</v>
+      </c>
+      <c r="H3" t="s">
         <v>795</v>
-      </c>
-      <c r="H3" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -7828,7 +7828,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G5" t="s">
         <v>662</v>
@@ -7839,7 +7839,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G6" t="s">
         <v>663</v>
@@ -7859,7 +7859,7 @@
         <v>669</v>
       </c>
       <c r="G10" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
@@ -7867,20 +7867,20 @@
         <v>359</v>
       </c>
       <c r="G11" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="G12" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G13" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="H13">
         <v>13889</v>
@@ -7888,10 +7888,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>717</v>
+        <v>990</v>
       </c>
       <c r="G14" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H14">
         <v>13889</v>
@@ -7899,7 +7899,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="G15" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H15" s="2">
         <f>H14/H13</f>
@@ -7908,7 +7908,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>